<commit_message>
Finishing touches for report
</commit_message>
<xml_diff>
--- a/Iridium Photocatalysts/Iridium photocatalyst summary statistics.xlsx
+++ b/Iridium Photocatalysts/Iridium photocatalyst summary statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubai\Documents\Programming\AI3SD\edbo\Iridium Photocatalysts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F63686-3B88-4BE6-BE54-A4A4843287E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD91831D-FD6C-4BCE-8BC1-220E4844BD3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{400A3B9E-BF8C-49BF-8024-4E4E65349EFC}"/>
   </bookViews>
@@ -1117,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B0C78E-B9DC-4ED7-B52B-2124B1D5F551}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1688,16 +1688,30 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
-        <f t="shared" ref="A53:B53" si="0">COUNTIF(A2:A51,2.675062079)</f>
+        <f>COUNTIF(A2:A51,$C$3)</f>
         <v>11</v>
       </c>
       <c r="B53">
+        <f t="shared" ref="B53:C53" si="0">COUNTIF(B2:B51,$C$3)</f>
+        <v>19</v>
+      </c>
+      <c r="C53">
         <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f>COUNTIF(A2:A51,$C$2)</f>
         <v>19</v>
       </c>
-      <c r="C53">
-        <f>COUNTIF(C2:C51,2.675062079)</f>
-        <v>23</v>
+      <c r="B54">
+        <f t="shared" ref="B54:C54" si="1">COUNTIF(B2:B51,$C$2)</f>
+        <v>28</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>